<commit_message>
DataProvider sheet path problem resolved
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/testData/testDATA.xlsx
+++ b/src/main/java/com/qa/testData/testDATA.xlsx
@@ -4,15 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="12240" windowHeight="3600"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="11400" windowHeight="2025"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="productData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:J5"/>
 </workbook>
 </file>
 
@@ -377,7 +375,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -417,28 +415,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>